<commit_message>
Updating RBD & LSD content as well as adding new data for HW1
</commit_message>
<xml_diff>
--- a/Assignments/HW1/IPA.xlsx
+++ b/Assignments/HW1/IPA.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>51.71</v>
+        <v>39.41</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>43.53</v>
+        <v>53.18</v>
       </c>
     </row>
     <row r="4">
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>47.25</v>
+        <v>35.31</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>41.57</v>
+        <v>59.62</v>
       </c>
     </row>
     <row r="6">
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>46.27</v>
+        <v>40.95</v>
       </c>
     </row>
     <row r="7">
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>44.04</v>
+        <v>47.79</v>
       </c>
     </row>
     <row r="8">
@@ -436,7 +436,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>44.47</v>
+        <v>56.88</v>
       </c>
     </row>
     <row r="9">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>57.75</v>
+        <v>48.39</v>
       </c>
     </row>
     <row r="10">
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>39.04</v>
+        <v>54.21</v>
       </c>
     </row>
     <row r="11">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>40.94</v>
+        <v>56.42</v>
       </c>
     </row>
     <row r="12">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>62.57</v>
+        <v>63.75</v>
       </c>
     </row>
     <row r="13">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>59.56</v>
+        <v>47.82</v>
       </c>
     </row>
     <row r="14">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>65.78</v>
+        <v>71.7</v>
       </c>
     </row>
     <row r="15">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>44.56</v>
+        <v>70.75</v>
       </c>
     </row>
     <row r="16">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>81.98999999999999</v>
+        <v>67.81</v>
       </c>
     </row>
     <row r="17">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>55.9</v>
+        <v>68.93000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>48.24</v>
+        <v>55.42</v>
       </c>
     </row>
     <row r="19">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>62.32</v>
+        <v>68.79000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>65.31</v>
+        <v>54.45</v>
       </c>
     </row>
     <row r="21">
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>55.41</v>
+        <v>58.09</v>
       </c>
     </row>
     <row r="22">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>48.93</v>
+        <v>61.66</v>
       </c>
     </row>
     <row r="23">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>65.8</v>
+        <v>78.03</v>
       </c>
     </row>
     <row r="24">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>84.22</v>
+        <v>71.78</v>
       </c>
     </row>
     <row r="25">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>61.82</v>
+        <v>70.12</v>
       </c>
     </row>
     <row r="26">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>68.28</v>
+        <v>73.56999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>81.31999999999999</v>
+        <v>72.06999999999999</v>
       </c>
     </row>
     <row r="28">
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>80.44</v>
+        <v>69.75</v>
       </c>
     </row>
     <row r="29">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>74.65000000000001</v>
+        <v>65.98999999999999</v>
       </c>
     </row>
     <row r="30">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>62.13</v>
+        <v>74.19</v>
       </c>
     </row>
     <row r="31">
@@ -666,7 +666,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>90.31999999999999</v>
+        <v>60.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>